<commit_message>
rendering the new added previous seminars
</commit_message>
<xml_diff>
--- a/docs/data/seminars.xlsx
+++ b/docs/data/seminars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novartisnam-my.sharepoint.com/personal/izemri1_novartis_net/Documents/MyRef/Training/BES/2023-10-23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\izemri1\Downloads\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{FD275AD2-67BE-46EE-B4C5-3DB380A3CCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98FD7F3F-B5CC-497D-B21A-F39A6964BE14}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DFF05E4-6B97-437C-8A36-C5BF6ED1133D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conferences" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
   <si>
     <t>date</t>
   </si>
@@ -121,6 +121,162 @@
   <si>
     <t>27.10.2023</t>
   </si>
+  <si>
+    <t>15.03.2023</t>
+  </si>
+  <si>
+    <t>Joint BES/BBS: RWD quality</t>
+  </si>
+  <si>
+    <t>Massoud Toussi</t>
+  </si>
+  <si>
+    <t>Nicole Mahoney</t>
+  </si>
+  <si>
+    <t>Clair Blacketer</t>
+  </si>
+  <si>
+    <t>Daniel Morales</t>
+  </si>
+  <si>
+    <t>Dalia Dawoud</t>
+  </si>
+  <si>
+    <t>Spencer James</t>
+  </si>
+  <si>
+    <t>Gracy Crane</t>
+  </si>
+  <si>
+    <t>Janssen</t>
+  </si>
+  <si>
+    <t>EMA</t>
+  </si>
+  <si>
+    <t>NICE</t>
+  </si>
+  <si>
+    <t>Roche/Genentech</t>
+  </si>
+  <si>
+    <t>What is data quality, and how data types differ in terms of data quality</t>
+  </si>
+  <si>
+    <t>RWD for regulatory decisions</t>
+  </si>
+  <si>
+    <t>EHDEN: Data Quality Dashboard</t>
+  </si>
+  <si>
+    <t>EU Data quality framework</t>
+  </si>
+  <si>
+    <t>COPD case study - The Use of OMOP Common DataModel in Health Technology Assessment</t>
+  </si>
+  <si>
+    <t>Data quality in Flatiron</t>
+  </si>
+  <si>
+    <t>Transcelerate - How to bridge from framework to fitness for purpose demonstration</t>
+  </si>
+  <si>
+    <t>1_Toussi.pdf</t>
+  </si>
+  <si>
+    <t>2_Mahoney.pdf</t>
+  </si>
+  <si>
+    <t>3_Blacketer.pdf</t>
+  </si>
+  <si>
+    <t>4_Morales.pdf</t>
+  </si>
+  <si>
+    <t>5_Dawoud.pdf</t>
+  </si>
+  <si>
+    <t>6_James.pdf</t>
+  </si>
+  <si>
+    <t>7_Crane.pdf</t>
+  </si>
+  <si>
+    <t>09.03.2018</t>
+  </si>
+  <si>
+    <t>Missing data - What can we do?</t>
+  </si>
+  <si>
+    <t>Christian Schindler</t>
+  </si>
+  <si>
+    <t>Audrey Muller</t>
+  </si>
+  <si>
+    <t>Actelion</t>
+  </si>
+  <si>
+    <t>SwissTPH</t>
+  </si>
+  <si>
+    <t>Overview of statistical methods used and envisaged to handle attrition bias in SAPALDIA</t>
+  </si>
+  <si>
+    <t>Comparative effectiveness in rare disease: Handling of missing data for propensity score use in EXPOSURE</t>
+  </si>
+  <si>
+    <t>Comparative effectiveness of patients with ALK-positive non-small-cell lung cancer following progression on crizotinib: a comparison of alectinib single-arm phase II data versus ceritinib real-world data</t>
+  </si>
+  <si>
+    <t>1_Schindler</t>
+  </si>
+  <si>
+    <t>2_Muller</t>
+  </si>
+  <si>
+    <t>3_Crane</t>
+  </si>
+  <si>
+    <t>23.06.2017</t>
+  </si>
+  <si>
+    <t>Challenges when studying associations between exposure and outcomes with long latencies</t>
+  </si>
+  <si>
+    <t>Christoph Meier</t>
+  </si>
+  <si>
+    <t>University of Basel</t>
+  </si>
+  <si>
+    <t>Sigrid Behr and Daniel Rosenberg</t>
+  </si>
+  <si>
+    <t>Novartis/Actelion</t>
+  </si>
+  <si>
+    <t>Anna Beckmeyer-Borowko</t>
+  </si>
+  <si>
+    <t>Case study of studying the association between benzodiazepines and Alzheimer's disease</t>
+  </si>
+  <si>
+    <t>Assessing long term latencies for newly marketed drugs: mission impossible for the epidemiologist</t>
+  </si>
+  <si>
+    <t>The value of population-based studies and their associated biobanks in studying long term exposure effects</t>
+  </si>
+  <si>
+    <t>1_Meier</t>
+  </si>
+  <si>
+    <t>2_Behr</t>
+  </si>
+  <si>
+    <t>3_Beckmeyer</t>
+  </si>
 </sst>
 </file>
 
@@ -129,7 +285,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -158,6 +314,10 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -321,10 +481,6 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,20 +750,20 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="8" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="186.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="187.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="8" customWidth="1"/>
     <col min="6" max="6" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="155.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="160" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="83.42578125" style="14" customWidth="1"/>
     <col min="10" max="10" width="64.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="73.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="14.42578125" style="7"/>
@@ -753,160 +909,342 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="15"/>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="15"/>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="15"/>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="15"/>
+      <c r="F9" s="3">
+        <v>4</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="15"/>
+      <c r="F10" s="3">
+        <v>5</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="12"/>
+      <c r="A11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="15"/>
+      <c r="F11" s="3">
+        <v>6</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="15"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="12"/>
+      <c r="F12" s="3">
+        <v>7</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="15"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="12"/>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="12"/>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="12"/>
+      <c r="F15" s="3">
+        <v>3</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="12"/>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="12"/>
+      <c r="F17" s="3">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="15"/>
+      <c r="F18" s="3">
+        <v>3</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
@@ -8481,6 +8819,7 @@
       <c r="J649" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update past events page with recent seminar
</commit_message>
<xml_diff>
--- a/docs/data/seminars.xlsx
+++ b/docs/data/seminars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\izemri1\Downloads\home\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://my.novartis.net/personal/behrsi1_novartis_net/Documents/_BACKUP H-Drive/QSE/BaselEpiSeminar/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DFF05E4-6B97-437C-8A36-C5BF6ED1133D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{7CA31F3F-8CCB-4474-99DA-51A60DBB2A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91870FB1-093B-4D07-B5D4-4CCE5E6DCBC9}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conferences" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
   <si>
     <t>date</t>
   </si>
@@ -276,6 +276,75 @@
   </si>
   <si>
     <t>3_Beckmeyer</t>
+  </si>
+  <si>
+    <t>Methods for rare diseases, small or special populations</t>
+  </si>
+  <si>
+    <t>Daniel Rosenberg</t>
+  </si>
+  <si>
+    <t>Johnson and Johnson</t>
+  </si>
+  <si>
+    <t>Rare diseases: Challenges to generate Real‐World Evidence</t>
+  </si>
+  <si>
+    <t>1_Rosenberg.pdf</t>
+  </si>
+  <si>
+    <t>Keith McDonald</t>
+  </si>
+  <si>
+    <t>Overview of the regulatory landscape for development of medicines intended for rare diseases</t>
+  </si>
+  <si>
+    <t>2_McDonald.pdf</t>
+  </si>
+  <si>
+    <t>Laura Girardat-Rotar</t>
+  </si>
+  <si>
+    <t>Multi‐regional, long‐term PASS using mixed data sources</t>
+  </si>
+  <si>
+    <t>3_GirardatRotar.pdf</t>
+  </si>
+  <si>
+    <t>Jilles Fermont</t>
+  </si>
+  <si>
+    <t>Collaborate to innovate: iptacopan and RWE in PNH treatment</t>
+  </si>
+  <si>
+    <t>4_Fermont.pdf</t>
+  </si>
+  <si>
+    <t>retention policy</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>remove 2 years after event</t>
+  </si>
+  <si>
+    <t>Challenges for comparative designs in rare diseases</t>
+  </si>
+  <si>
+    <t>5_Muller.pdf</t>
+  </si>
+  <si>
+    <t>Maria Luisa Faquetti</t>
+  </si>
+  <si>
+    <t>ETH Zurich</t>
+  </si>
+  <si>
+    <t>Exploring the Applicability of the Prevalent New User Design in Rare Diseases</t>
+  </si>
+  <si>
+    <t>6_Faquetti.pdf</t>
   </si>
 </sst>
 </file>
@@ -285,7 +354,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -319,6 +388,12 @@
       <sz val="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -341,7 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -388,6 +463,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -412,7 +493,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -446,7 +527,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -746,11 +827,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K649"/>
+  <dimension ref="A1:L655"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +850,7 @@
     <col min="12" max="16384" width="14.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -803,268 +884,301 @@
       <c r="K1" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="L1" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="16">
+        <v>45456</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>45456</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>45456</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="16">
+        <v>45456</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
+        <v>45456</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="16">
+        <v>45456</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7">
+      <c r="C8" s="3"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="L8" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7">
+      <c r="C9" s="3"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7">
         <v>2</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="L9" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7">
+      <c r="C10" s="3"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J10" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="L10" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7">
+      <c r="C11" s="3"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7">
         <v>4</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="3">
-        <v>2</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="3">
-        <v>3</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="3">
-        <v>4</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="3">
-        <v>5</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="3">
-        <v>6</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
@@ -1075,250 +1189,373 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="28.5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="12"/>
+        <v>55</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="12"/>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="15"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="12"/>
+      <c r="F20" s="3">
+        <v>2</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="12"/>
+      <c r="F21" s="3">
+        <v>3</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="15"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="12"/>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="12"/>
+      <c r="F23" s="3">
+        <v>2</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="15"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="3">
+        <v>3</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="12"/>
       <c r="C25" s="11"/>
@@ -1330,7 +1567,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="15"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="12"/>
       <c r="C26" s="11"/>
@@ -1342,7 +1579,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="12"/>
       <c r="C27" s="11"/>
@@ -1354,7 +1591,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="15"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="12"/>
       <c r="C28" s="11"/>
@@ -1366,7 +1603,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="15"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="12"/>
       <c r="C29" s="11"/>
@@ -1378,7 +1615,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="15"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="12"/>
       <c r="C30" s="11"/>
@@ -1390,7 +1627,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="15"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="12"/>
       <c r="C31" s="11"/>
@@ -1402,7 +1639,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="15"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="12"/>
       <c r="C32" s="11"/>
@@ -2303,76 +2540,76 @@
       <c r="J106" s="15"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="10"/>
-      <c r="B107" s="6"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="2"/>
+      <c r="A107" s="9"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="3"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="2"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="15"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="10"/>
-      <c r="B108" s="6"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="2"/>
+      <c r="A108" s="9"/>
+      <c r="B108" s="12"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="3"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="2"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="15"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="10"/>
-      <c r="B109" s="6"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="2"/>
+      <c r="A109" s="9"/>
+      <c r="B109" s="12"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="3"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
-      <c r="I109" s="13"/>
-      <c r="J109" s="2"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="15"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="10"/>
-      <c r="B110" s="6"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="2"/>
+      <c r="A110" s="9"/>
+      <c r="B110" s="12"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="3"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
-      <c r="I110" s="13"/>
-      <c r="J110" s="2"/>
+      <c r="I110" s="1"/>
+      <c r="J110" s="15"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="10"/>
-      <c r="B111" s="6"/>
-      <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="2"/>
+      <c r="A111" s="9"/>
+      <c r="B111" s="12"/>
+      <c r="C111" s="11"/>
+      <c r="D111" s="11"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="3"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
-      <c r="I111" s="13"/>
-      <c r="J111" s="2"/>
+      <c r="I111" s="1"/>
+      <c r="J111" s="15"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="10"/>
-      <c r="B112" s="6"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="2"/>
+      <c r="A112" s="9"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="3"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
-      <c r="I112" s="13"/>
-      <c r="J112" s="2"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="15"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
@@ -8818,6 +9055,78 @@
       <c r="I649" s="13"/>
       <c r="J649" s="2"/>
     </row>
+    <row r="650" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A650" s="10"/>
+      <c r="B650" s="6"/>
+      <c r="C650" s="4"/>
+      <c r="D650" s="4"/>
+      <c r="E650" s="4"/>
+      <c r="F650" s="2"/>
+      <c r="G650" s="4"/>
+      <c r="H650" s="4"/>
+      <c r="I650" s="13"/>
+      <c r="J650" s="2"/>
+    </row>
+    <row r="651" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A651" s="10"/>
+      <c r="B651" s="6"/>
+      <c r="C651" s="4"/>
+      <c r="D651" s="4"/>
+      <c r="E651" s="4"/>
+      <c r="F651" s="2"/>
+      <c r="G651" s="4"/>
+      <c r="H651" s="4"/>
+      <c r="I651" s="13"/>
+      <c r="J651" s="2"/>
+    </row>
+    <row r="652" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A652" s="10"/>
+      <c r="B652" s="6"/>
+      <c r="C652" s="4"/>
+      <c r="D652" s="4"/>
+      <c r="E652" s="4"/>
+      <c r="F652" s="2"/>
+      <c r="G652" s="4"/>
+      <c r="H652" s="4"/>
+      <c r="I652" s="13"/>
+      <c r="J652" s="2"/>
+    </row>
+    <row r="653" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A653" s="10"/>
+      <c r="B653" s="6"/>
+      <c r="C653" s="4"/>
+      <c r="D653" s="4"/>
+      <c r="E653" s="4"/>
+      <c r="F653" s="2"/>
+      <c r="G653" s="4"/>
+      <c r="H653" s="4"/>
+      <c r="I653" s="13"/>
+      <c r="J653" s="2"/>
+    </row>
+    <row r="654" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A654" s="10"/>
+      <c r="B654" s="6"/>
+      <c r="C654" s="4"/>
+      <c r="D654" s="4"/>
+      <c r="E654" s="4"/>
+      <c r="F654" s="2"/>
+      <c r="G654" s="4"/>
+      <c r="H654" s="4"/>
+      <c r="I654" s="13"/>
+      <c r="J654" s="2"/>
+    </row>
+    <row r="655" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A655" s="10"/>
+      <c r="B655" s="6"/>
+      <c r="C655" s="4"/>
+      <c r="D655" s="4"/>
+      <c r="E655" s="4"/>
+      <c r="F655" s="2"/>
+      <c r="G655" s="4"/>
+      <c r="H655" s="4"/>
+      <c r="I655" s="13"/>
+      <c r="J655" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>